<commit_message>
added aggregate.xlsx and aggregate.csv data files to data folder
</commit_message>
<xml_diff>
--- a/data/aggregate.xlsx
+++ b/data/aggregate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conny\Desktop\Computerlinguistik\Semester 8\Tabellen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91269D73-2782-40EC-B2DC-81575A77DD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DACB565-5D8A-4D75-AE0A-B40C0E727B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{53178692-CF69-473C-8C63-3A27B49975ED}"/>
   </bookViews>
@@ -391,7 +391,7 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>